<commit_message>
added first version of class 'OrientedGraph' and changed file with tasks
</commit_message>
<xml_diff>
--- a/Current Tasks Backlog.xlsx
+++ b/Current Tasks Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Priority</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Client-Server</t>
+  </si>
+  <si>
+    <t>Kochetov Pavel</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -449,6 +452,9 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">

</xml_diff>

<commit_message>
changed file of tasks
</commit_message>
<xml_diff>
--- a/Current Tasks Backlog.xlsx
+++ b/Current Tasks Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Priority</t>
   </si>
@@ -415,7 +415,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -463,6 +463,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">

</xml_diff>

<commit_message>
No bugs (I hope).
</commit_message>
<xml_diff>
--- a/Current Tasks Backlog.xlsx
+++ b/Current Tasks Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Priority</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Flowchart to code functionality (pizdos)</t>
   </si>
   <si>
-    <t>Google about libraries for code parsing</t>
-  </si>
-  <si>
-    <t>ViewModel</t>
-  </si>
-  <si>
     <t>View</t>
   </si>
   <si>
@@ -58,6 +52,45 @@
   </si>
   <si>
     <t>Client-Server</t>
+  </si>
+  <si>
+    <t>Кочетов</t>
+  </si>
+  <si>
+    <t>Чугунов</t>
+  </si>
+  <si>
+    <t>Взаимодействие с презентером</t>
+  </si>
+  <si>
+    <t>Презентер</t>
+  </si>
+  <si>
+    <t>Веселов</t>
+  </si>
+  <si>
+    <t>Взаимодействие со вьюхами</t>
+  </si>
+  <si>
+    <t>Построение модели</t>
+  </si>
+  <si>
+    <t>Отрисовка всего</t>
+  </si>
+  <si>
+    <t>Поддержка моделью координат</t>
+  </si>
+  <si>
+    <t>Класс управление БД</t>
+  </si>
+  <si>
+    <t>Реакция вьюхи на мелкие вещи ()</t>
+  </si>
+  <si>
+    <t>Веселов/Кочетов</t>
+  </si>
+  <si>
+    <t>Взаимодействие с моделью</t>
   </si>
 </sst>
 </file>
@@ -113,8 +146,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:C25" totalsRowShown="0">
-  <autoFilter ref="A1:C25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:C35" totalsRowShown="0">
+  <autoFilter ref="A1:C35"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Priority"/>
     <tableColumn id="2" name="Task"/>
@@ -409,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -449,6 +482,9 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
@@ -457,6 +493,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
@@ -465,6 +504,9 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
@@ -476,55 +518,117 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1"/>
+      <c r="C35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>